<commit_message>
Moving data and adding data for revenue
</commit_message>
<xml_diff>
--- a/Apps/YouTubeAnalysis/Analysis/Content/Step03_GroupByClassification.xlsx
+++ b/Apps/YouTubeAnalysis/Analysis/Content/Step03_GroupByClassification.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0"/>
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="17" uniqueCount="17">
   <si>
     <t>Classification</t>
   </si>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -108,25 +108,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.984375" customWidth="true"/>
-    <col min="2" max="2" width="17.7109375" customWidth="true"/>
-    <col min="3" max="3" width="10.16796875" customWidth="true"/>
-    <col min="4" max="4" width="17.62109375" customWidth="true"/>
-    <col min="5" max="5" width="14.89453125" customWidth="true"/>
-    <col min="6" max="6" width="16.984375" customWidth="true"/>
-    <col min="7" max="7" width="15.44140625" customWidth="true"/>
-    <col min="8" max="8" width="20.2578125" customWidth="true"/>
-    <col min="9" max="9" width="27.984375" customWidth="true"/>
-    <col min="10" max="10" width="20.44140625" customWidth="true"/>
-    <col min="11" max="11" width="27.89453125" customWidth="true"/>
-    <col min="12" max="12" width="25.16796875" customWidth="true"/>
-    <col min="13" max="13" width="27.2578125" customWidth="true"/>
-    <col min="14" max="14" width="25.7109375" customWidth="true"/>
-    <col min="15" max="15" width="30.53125" customWidth="true"/>
+    <col min="1" max="1" width="12.85546875" customWidth="true"/>
+    <col min="2" max="2" width="19" customWidth="true"/>
+    <col min="3" max="3" width="11" customWidth="true"/>
+    <col min="4" max="4" width="18.42578125" customWidth="true"/>
+    <col min="5" max="5" width="15.7109375" customWidth="true"/>
+    <col min="6" max="6" width="18" customWidth="true"/>
+    <col min="7" max="7" width="16.28515625" customWidth="true"/>
+    <col min="8" max="8" width="21.42578125" customWidth="true"/>
+    <col min="9" max="9" width="30" customWidth="true"/>
+    <col min="10" max="10" width="22" customWidth="true"/>
+    <col min="11" max="11" width="29.42578125" customWidth="true"/>
+    <col min="12" max="12" width="26.7109375" customWidth="true"/>
+    <col min="13" max="13" width="29" customWidth="true"/>
+    <col min="14" max="14" width="27.28515625" customWidth="true"/>
+    <col min="15" max="15" width="32.42578125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Updates to YouTube app to get revenue
</commit_message>
<xml_diff>
--- a/Apps/YouTubeAnalysis/Analysis/Content/Step03_GroupByClassification.xlsx
+++ b/Apps/YouTubeAnalysis/Analysis/Content/Step03_GroupByClassification.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0"/>
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Classification</t>
   </si>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -108,28 +108,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="true"/>
-    <col min="2" max="2" width="19" customWidth="true"/>
-    <col min="3" max="3" width="11" customWidth="true"/>
-    <col min="4" max="4" width="18.42578125" customWidth="true"/>
-    <col min="5" max="5" width="15.7109375" customWidth="true"/>
-    <col min="6" max="6" width="18" customWidth="true"/>
-    <col min="7" max="7" width="16.28515625" customWidth="true"/>
-    <col min="8" max="8" width="21.42578125" customWidth="true"/>
-    <col min="9" max="9" width="30" customWidth="true"/>
-    <col min="10" max="10" width="22" customWidth="true"/>
-    <col min="11" max="11" width="29.42578125" customWidth="true"/>
-    <col min="12" max="12" width="26.7109375" customWidth="true"/>
-    <col min="13" max="13" width="29" customWidth="true"/>
-    <col min="14" max="14" width="27.28515625" customWidth="true"/>
-    <col min="15" max="15" width="32.42578125" customWidth="true"/>
+    <col min="1" max="1" width="11.984375" customWidth="true"/>
+    <col min="2" max="2" width="17.7109375" customWidth="true"/>
+    <col min="3" max="3" width="10.16796875" customWidth="true"/>
+    <col min="4" max="4" width="17.62109375" customWidth="true"/>
+    <col min="5" max="5" width="14.89453125" customWidth="true"/>
+    <col min="6" max="6" width="16.984375" customWidth="true"/>
+    <col min="7" max="7" width="15.44140625" customWidth="true"/>
+    <col min="8" max="8" width="20.2578125" customWidth="true"/>
+    <col min="9" max="9" width="27.984375" customWidth="true"/>
+    <col min="10" max="10" width="20.44140625" customWidth="true"/>
+    <col min="11" max="11" width="27.89453125" customWidth="true"/>
+    <col min="12" max="12" width="25.16796875" customWidth="true"/>
+    <col min="13" max="13" width="27.2578125" customWidth="true"/>
+    <col min="14" max="14" width="25.7109375" customWidth="true"/>
+    <col min="15" max="15" width="30.53125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>